<commit_message>
show record duplicate in progress 05
</commit_message>
<xml_diff>
--- a/uploads/00 BHA-BPRM_Base Registro Nacional_stage_upload_200_casos.xlsx
+++ b/uploads/00 BHA-BPRM_Base Registro Nacional_stage_upload_200_casos.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13232" uniqueCount="2885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13239" uniqueCount="2885">
   <si>
     <t>2021-09-15</t>
   </si>
@@ -9145,8 +9145,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:EN201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A201" sqref="A201:EM201"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BU33" sqref="BU33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12194,7 +12194,7 @@
         <v>40</v>
       </c>
       <c r="CF12" t="s">
-        <v>350</v>
+        <v>181</v>
       </c>
       <c r="EG12" t="s">
         <v>5</v>
@@ -16205,6 +16205,27 @@
       </c>
       <c r="BK31" t="s">
         <v>26</v>
+      </c>
+      <c r="BM31" t="s">
+        <v>160</v>
+      </c>
+      <c r="BN31" t="s">
+        <v>161</v>
+      </c>
+      <c r="BQ31" t="s">
+        <v>12</v>
+      </c>
+      <c r="BR31" t="s">
+        <v>164</v>
+      </c>
+      <c r="BS31" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU31" t="s">
+        <v>68</v>
+      </c>
+      <c r="BV31" t="s">
+        <v>165</v>
       </c>
       <c r="EG31" t="s">
         <v>5</v>

</xml_diff>